<commit_message>
added Current Fiscal Year To Excel
</commit_message>
<xml_diff>
--- a/fakedata/Brandeis_ClipperShipGrant_2023 .xlsx
+++ b/fakedata/Brandeis_ClipperShipGrant_2023 .xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnL\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB18B2C-B67C-4281-8AFA-0760A09536BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Questions" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Clipper Ship Standardized Excel Sheet</t>
   </si>
@@ -114,51 +123,58 @@
   </si>
   <si>
     <t>Please indicate the amount of funding Clipper Ship has awarded to your organization in FY' 21:</t>
+  </si>
+  <si>
+    <t>Current Fiscal Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -168,70 +184,59 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -421,49 +426,54 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="120.0"/>
-    <col customWidth="1" min="2" max="2" width="16.25"/>
+    <col min="1" max="1" width="120" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -471,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -479,7 +489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -487,173 +497,182 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8">
-        <v>2000.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="8">
-        <v>1800.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="B13" s="7">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="4">
-        <v>150.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="4">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="4">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="10"/>
-    </row>
-    <row r="19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="161.5"/>
+    <col min="1" max="1" width="161.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>